<commit_message>
Added XL module starting point
</commit_message>
<xml_diff>
--- a/24-0005E2.xlsx
+++ b/24-0005E2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aro365534042-my.sharepoint.com/personal/abarnes_psconline_net/Documents/Documents/Panel Building/Labels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndrewBarnes\Downloads\PSC-XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{0042B06C-BA35-4DFD-9836-D27E11153A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5424F59-164D-435D-BD12-90098DE56B2F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2600227-BD56-4697-98A0-E2F9968B3AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -512,20 +512,20 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -548,10 +548,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -841,241 +837,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:A58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="A49" sqref="A49:A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="2" t="s">
+    </row>
+    <row r="32" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="E11" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="E12" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C31" s="2"/>
+    <row r="58" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1723,100 +1781,100 @@
       <c r="A14" s="11"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
+      <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
+      <c r="A18" s="13"/>
     </row>
     <row r="19" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
+      <c r="A20" s="13"/>
     </row>
     <row r="21" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
+      <c r="A22" s="12"/>
     </row>
     <row r="23" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
+      <c r="A24" s="12"/>
     </row>
     <row r="25" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="12" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
+      <c r="A26" s="12"/>
     </row>
     <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
+      <c r="A28" s="12"/>
     </row>
     <row r="29" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
+      <c r="A30" s="12"/>
     </row>
     <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="12" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
+      <c r="A32" s="12"/>
     </row>
     <row r="33" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
+      <c r="A34" s="12"/>
     </row>
     <row r="35" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
+      <c r="A36" s="12"/>
     </row>
     <row r="37" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="12" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="10"/>
+      <c r="A38" s="12"/>
     </row>
     <row r="39" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
@@ -1877,28 +1935,28 @@
       <c r="A52" s="9"/>
     </row>
     <row r="53" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="10" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="14"/>
+      <c r="A54" s="10"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14" t="s">
+      <c r="A55" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
+      <c r="A56" s="10"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
+      <c r="A58" s="10"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
@@ -1917,12 +1975,12 @@
       <c r="A62" s="9"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="10" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="14"/>
+      <c r="A64" s="10"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
@@ -1958,16 +2016,13 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A41:A42"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="A51:A52"/>
@@ -1984,13 +2039,16 @@
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0.05" bottom="0" header="0" footer="0"/>

</xml_diff>